<commit_message>
Add cofigurable Start ID for DocumentRescources
</commit_message>
<xml_diff>
--- a/input/FHIR_Testdatengenerator_Vorlage.xlsx
+++ b/input/FHIR_Testdatengenerator_Vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\TestDataGenerator_MIIGitHub\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BED481-AFB8-456D-8C7C-91566FDD9C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD81475-93B6-4318-9675-88F67F290CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Medikation!$D$1:$D$897</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -89,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="1130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="1131">
   <si>
     <t>Patient-ID</t>
   </si>
@@ -3479,6 +3478,9 @@
   </si>
   <si>
     <t xml:space="preserve"># </t>
+  </si>
+  <si>
+    <t>#START_ID_DOCUMENT_REFERENCE = 1</t>
   </si>
 </sst>
 </file>
@@ -8008,10 +8010,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B0353-4A30-49CF-9E96-AB439FF3F972}">
-  <dimension ref="A1:A152"/>
+  <dimension ref="A1:A153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -8149,559 +8151,564 @@
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="48"/>
+      <c r="A27" s="48" t="s">
+        <v>1130</v>
+      </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="48"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="48" t="s">
-        <v>909</v>
-      </c>
+      <c r="A29" s="48"/>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="48" t="s">
-        <v>999</v>
+        <v>909</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="48" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="48" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="48" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="50" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" s="50" t="s">
         <v>1001</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="48"/>
-    </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="48" t="s">
-        <v>909</v>
-      </c>
+      <c r="A35" s="48"/>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="48" t="s">
-        <v>1002</v>
+        <v>909</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="48" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="48" t="s">
-        <v>909</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="48" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="48" t="s">
         <v>1003</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="48"/>
-    </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="48" t="s">
-        <v>909</v>
-      </c>
+      <c r="A41" s="48"/>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="48" t="s">
-        <v>976</v>
+        <v>909</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="48" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="48" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="48" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="48" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="49" t="s">
+    <row r="47" spans="1:1">
+      <c r="A47" s="49" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="51" t="s">
+    <row r="48" spans="1:1">
+      <c r="A48" s="51" t="s">
         <v>980</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="49" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="49" t="s">
-        <v>976</v>
+        <v>909</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="49" t="s">
-        <v>981</v>
+        <v>976</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="49" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="49" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="49" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="49" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="49" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="51" t="s">
+    <row r="57" spans="1:1">
+      <c r="A57" s="51" t="s">
         <v>985</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="49" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="49" t="s">
-        <v>986</v>
+        <v>909</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="49" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="49" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="49" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="49" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="51" t="s">
+    <row r="64" spans="1:1">
+      <c r="A64" s="51" t="s">
         <v>989</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="49" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="49" t="s">
-        <v>932</v>
+        <v>909</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="49" t="s">
-        <v>948</v>
+        <v>932</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="49" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="49" t="s">
-        <v>949</v>
+        <v>940</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="49" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="49" t="s">
-        <v>933</v>
+        <v>950</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="49" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="49" t="s">
-        <v>951</v>
+        <v>934</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="49" t="s">
-        <v>935</v>
+        <v>951</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="49" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="49" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="49" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="51" t="s">
+    <row r="79" spans="1:1">
+      <c r="A79" s="51" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="49" t="s">
+    <row r="80" spans="1:1">
+      <c r="A80" s="49" t="s">
         <v>937</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="49" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="49" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="49" t="s">
-        <v>952</v>
+        <v>939</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="49" t="s">
-        <v>940</v>
+        <v>952</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="49" t="s">
-        <v>953</v>
+        <v>940</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="49" t="s">
-        <v>941</v>
+        <v>953</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="49" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="49" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="49" t="s">
-        <v>954</v>
+        <v>943</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="49" t="s">
-        <v>935</v>
+        <v>954</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="49" t="s">
-        <v>944</v>
+        <v>935</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="49" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="49" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="51" t="s">
+    <row r="94" spans="1:1">
+      <c r="A94" s="51" t="s">
         <v>955</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" s="49" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="49" t="s">
-        <v>932</v>
+        <v>909</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="49" t="s">
-        <v>956</v>
+        <v>932</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="49" t="s">
-        <v>940</v>
+        <v>956</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="49" t="s">
-        <v>949</v>
+        <v>940</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="49" t="s">
-        <v>957</v>
+        <v>949</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="49" t="s">
-        <v>933</v>
+        <v>957</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="49" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="49" t="s">
-        <v>958</v>
+        <v>934</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="49" t="s">
-        <v>935</v>
+        <v>958</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="49" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="49" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="49" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
-      <c r="A108" s="51" t="s">
+    <row r="109" spans="1:1">
+      <c r="A109" s="51" t="s">
         <v>959</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
-      <c r="A109" s="49" t="s">
+    <row r="110" spans="1:1">
+      <c r="A110" s="49" t="s">
         <v>937</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" s="49" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="49" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="49" t="s">
-        <v>960</v>
+        <v>939</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="49" t="s">
-        <v>940</v>
+        <v>960</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="49" t="s">
-        <v>961</v>
+        <v>940</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="49" t="s">
-        <v>941</v>
+        <v>961</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="49" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" s="49" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="49" t="s">
-        <v>962</v>
+        <v>943</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" s="49" t="s">
-        <v>935</v>
+        <v>962</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="49" t="s">
-        <v>944</v>
+        <v>935</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" s="49" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="49" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
-      <c r="A123" s="51" t="s">
+    <row r="124" spans="1:1">
+      <c r="A124" s="51" t="s">
         <v>963</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1">
-      <c r="A126" s="49" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" s="49" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" s="49" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="49" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="49" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" s="49" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" s="49" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="49" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" s="49" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="49" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" s="49" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="49" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
-      <c r="A137" s="51" t="s">
+    <row r="138" spans="1:1">
+      <c r="A138" s="51" t="s">
         <v>945</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1">
-      <c r="A140" s="49" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" s="49" t="s">
-        <v>920</v>
+        <v>909</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" s="49" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" s="49" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" s="49" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" s="49" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" s="49" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" s="49" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" s="49" t="s">
-        <v>919</v>
+        <v>926</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" s="49" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="49" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
-      <c r="A150" s="51" t="s">
+    <row r="151" spans="1:1">
+      <c r="A151" s="51" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
-      <c r="A152" s="49" t="s">
+    <row r="153" spans="1:1">
+      <c r="A153" s="49" t="s">
         <v>1129</v>
       </c>
     </row>

</xml_diff>